<commit_message>
* Read, Write implementation
</commit_message>
<xml_diff>
--- a/Sample/Test.xlsx
+++ b/Sample/Test.xlsx
@@ -345,12 +345,12 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>3.123</v>
-      </c>
-      <c r="E5" s="1" t="b">
+        <v>-3.1111</v>
+      </c>
+      <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -364,10 +364,10 @@
       <c r="C6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>4.555</v>
-      </c>
-      <c r="E6" s="1" t="b">
+      <c r="D6" s="1">
+        <v/>
+      </c>
+      <c r="E6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -384,8 +384,8 @@
       <c r="D7" s="1" t="n">
         <v>6.111</v>
       </c>
-      <c r="E7" s="1" t="b">
-        <v>1</v>
+      <c r="E7" s="1">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Load and save for multi-sheets
* Change core source directory
* Refactoring
</commit_message>
<xml_diff>
--- a/Sample/Test.xlsx
+++ b/Sample/Test.xlsx
@@ -3,6 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId3"/>
+    <sheet name="시트 2" sheetId="2" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <t>vv</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -91,11 +98,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -392,4 +402,46 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.299986" footer="0.299986"/>
   <extLst/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.299986" footer="0.299986"/>
+  <extLst/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
* Write file as UTF8 encoding
</commit_message>
<xml_diff>
--- a/Sample/Test.xlsx
+++ b/Sample/Test.xlsx
@@ -3,7 +3,6 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId3"/>
-    <sheet name="시트 2" sheetId="2" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -17,13 +16,16 @@
     <t>name</t>
   </si>
   <si>
-    <t>value</t>
+    <t>어머나</t>
+  </si>
+  <si>
+    <t>안녕</t>
   </si>
   <si>
     <t>float_val</t>
   </si>
   <si>
-    <t>bool_val</t>
+    <t>闪避</t>
   </si>
   <si>
     <t>int</t>
@@ -32,6 +34,9 @@
     <t>string</t>
   </si>
   <si>
+    <t>comment</t>
+  </si>
+  <si>
     <t>float</t>
   </si>
   <si>
@@ -44,19 +49,13 @@
     <t>D E F</t>
   </si>
   <si>
+    <t>攻击</t>
+  </si>
+  <si>
     <t>AB!@</t>
   </si>
   <si>
-    <t>안녕</t>
-  </si>
-  <si>
     <t>Hello</t>
-  </si>
-  <si>
-    <t>vv</t>
-  </si>
-  <si>
-    <t>v</t>
   </si>
 </sst>
 </file>
@@ -98,14 +97,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -273,7 +269,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -295,22 +291,28 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -318,15 +320,18 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="E3" s="1" t="b">
+      <c r="F3" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -335,15 +340,18 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="n">
         <v>2.11</v>
       </c>
-      <c r="E4" s="1" t="b">
+      <c r="F4" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -352,15 +360,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>-3</v>
       </c>
       <c r="D5" s="1" t="n">
+        <v>2345</v>
+      </c>
+      <c r="E5" s="1" t="n">
         <v>-3.1111</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="F5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -369,15 +380,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="n">
+        <v>9999</v>
+      </c>
+      <c r="E6" s="1">
         <v/>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="F6" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -386,58 +400,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="n">
+        <v>1111</v>
+      </c>
+      <c r="E7" s="1" t="n">
         <v>6.111</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.299986" footer="0.299986"/>
-  <extLst/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>